<commit_message>
2024-05-30: Change column for Images, OrderDetails table
</commit_message>
<xml_diff>
--- a/Database_Table.xlsx
+++ b/Database_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Sale_Shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DAB7B4-3E7E-4B33-9F4D-E29BCC488A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F716FE5-87A6-4F19-B15B-0992C29D993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9E4F9934-B007-48BA-86B0-9A5F347D8823}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -150,9 +150,6 @@
     <t>createat</t>
   </si>
   <si>
-    <t>size</t>
-  </si>
-  <si>
     <t>subtotal</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>FK(Products)</t>
   </si>
 </sst>
 </file>
@@ -243,10 +243,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -602,7 +601,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -622,7 +621,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -642,10 +641,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
@@ -676,7 +675,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -696,14 +695,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -716,16 +715,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -752,7 +751,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -772,14 +771,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -792,16 +791,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -822,14 +821,14 @@
     <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.6328125" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -842,58 +841,60 @@
         <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="4" t="s">
-        <v>38</v>
+      <c r="G3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +924,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -955,7 +956,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -968,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -987,10 +988,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
@@ -1000,7 +1001,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1032,7 +1033,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1049,7 +1050,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1066,10 +1067,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
@@ -1097,7 +1098,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1106,12 +1107,12 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1120,19 +1121,19 @@
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1164,7 +1165,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1194,12 +1195,12 @@
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1229,15 +1230,15 @@
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1"/>
@@ -1248,7 +1249,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2024-08-29: Change data type of phone from integer to varchar
</commit_message>
<xml_diff>
--- a/Database_Table.xlsx
+++ b/Database_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Sale_Shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F716FE5-87A6-4F19-B15B-0992C29D993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3B5E0C-2C9A-46DB-B6E8-E03D75FDDF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9E4F9934-B007-48BA-86B0-9A5F347D8823}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="7" xr2:uid="{9E4F9934-B007-48BA-86B0-9A5F347D8823}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>FK(Products)</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1147,7 +1150,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1213,7 +1218,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>16</v>

</xml_diff>